<commit_message>
rebuild files as classes
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reese.a.gallagher\PythonAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400D3CBF-D6F7-4D68-A9B1-62B555C06C3E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0C3C0D-BE29-473C-98FA-64CF1956905E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserTable" sheetId="1" r:id="rId1"/>
@@ -31,36 +31,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Frank</t>
-  </si>
-  <si>
-    <t>Sally</t>
-  </si>
-  <si>
     <t>user_name</t>
   </si>
   <si>
     <t>site</t>
   </si>
   <si>
-    <t>Lake Mary</t>
-  </si>
-  <si>
-    <t>Winter Park</t>
-  </si>
-  <si>
-    <t>Sanford</t>
-  </si>
-  <si>
     <t>group_id</t>
   </si>
   <si>
@@ -73,25 +49,49 @@
     <t>role_name</t>
   </si>
   <si>
-    <t>chemist</t>
-  </si>
-  <si>
-    <t>biologist</t>
-  </si>
-  <si>
-    <t>analyst</t>
-  </si>
-  <si>
-    <t>TeamExtreme</t>
-  </si>
-  <si>
-    <t>Lab42</t>
-  </si>
-  <si>
-    <t>Misfits</t>
-  </si>
-  <si>
     <t>username</t>
+  </si>
+  <si>
+    <t>"Bob"</t>
+  </si>
+  <si>
+    <t>"Mary"</t>
+  </si>
+  <si>
+    <t>"John"</t>
+  </si>
+  <si>
+    <t>"Frank"</t>
+  </si>
+  <si>
+    <t>"Sally"</t>
+  </si>
+  <si>
+    <t>"Lake Mary"</t>
+  </si>
+  <si>
+    <t>"Winter Park"</t>
+  </si>
+  <si>
+    <t>"Sanford"</t>
+  </si>
+  <si>
+    <t>"TeamExtreme"</t>
+  </si>
+  <si>
+    <t>"Lab42"</t>
+  </si>
+  <si>
+    <t>"Misfits"</t>
+  </si>
+  <si>
+    <t>"chemist"</t>
+  </si>
+  <si>
+    <t>"biologist"</t>
+  </si>
+  <si>
+    <t>"analyst"</t>
   </si>
 </sst>
 </file>
@@ -193,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -217,6 +217,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -501,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -517,50 +520,50 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+      <c r="A2" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
+      <c r="A3" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -574,7 +577,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -585,10 +588,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -596,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -604,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -612,7 +615,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -626,7 +629,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,15 +640,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>2</v>
@@ -653,7 +656,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -661,7 +664,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -669,7 +672,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
@@ -677,7 +680,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -685,7 +688,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -693,7 +696,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2">
         <v>3</v>
@@ -701,7 +704,7 @@
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
@@ -718,7 +721,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,10 +731,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -739,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -747,7 +750,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -755,7 +758,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -768,23 +771,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B42B11-64CF-4B94-9EA4-EE97BB3818C5}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -792,7 +795,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -800,7 +803,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -808,7 +811,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -816,7 +819,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
@@ -824,7 +827,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -832,7 +835,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -840,7 +843,7 @@
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>

</xml_diff>

<commit_message>
added type inference and main file
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reese.a.gallagher\PythonAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0C3C0D-BE29-473C-98FA-64CF1956905E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597675A1-152F-4018-98DC-E8599F2B7252}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4150" yWindow="2550" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserTable" sheetId="1" r:id="rId1"/>
@@ -504,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF9762C-F16D-4AB8-934C-C2B5D4F59B0D}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
In excel file columns, strings no longer need quotations, program can type deduce now.
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reese.a.gallagher\PythonAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597675A1-152F-4018-98DC-E8599F2B7252}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA270AD6-BE61-4A3B-B862-5D4D7AC15AD7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4150" yWindow="2550" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserTable" sheetId="1" r:id="rId1"/>
@@ -52,46 +52,46 @@
     <t>username</t>
   </si>
   <si>
-    <t>"Bob"</t>
-  </si>
-  <si>
-    <t>"Mary"</t>
-  </si>
-  <si>
-    <t>"John"</t>
-  </si>
-  <si>
-    <t>"Frank"</t>
-  </si>
-  <si>
-    <t>"Sally"</t>
-  </si>
-  <si>
-    <t>"Lake Mary"</t>
-  </si>
-  <si>
-    <t>"Winter Park"</t>
-  </si>
-  <si>
-    <t>"Sanford"</t>
-  </si>
-  <si>
-    <t>"TeamExtreme"</t>
-  </si>
-  <si>
-    <t>"Lab42"</t>
-  </si>
-  <si>
-    <t>"Misfits"</t>
-  </si>
-  <si>
-    <t>"chemist"</t>
-  </si>
-  <si>
-    <t>"biologist"</t>
-  </si>
-  <si>
-    <t>"analyst"</t>
+    <t>3TeamExtreme</t>
+  </si>
+  <si>
+    <t>Lab42</t>
+  </si>
+  <si>
+    <t>Misfits</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>Sally</t>
+  </si>
+  <si>
+    <t>Lake Mary</t>
+  </si>
+  <si>
+    <t>Sanford</t>
+  </si>
+  <si>
+    <t>Chemist</t>
+  </si>
+  <si>
+    <t>Biologist</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Winter Park</t>
   </si>
 </sst>
 </file>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,42 +528,42 @@
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -576,14 +576,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF9762C-F16D-4AB8-934C-C2B5D4F59B0D}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -599,7 +599,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -607,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -615,7 +615,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -629,7 +629,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -648,7 +648,7 @@
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>2</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -696,7 +696,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2">
         <v>3</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
@@ -721,7 +721,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -750,7 +750,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -758,7 +758,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +772,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -787,7 +787,7 @@
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>

</xml_diff>